<commit_message>
Added basic change plot
</commit_message>
<xml_diff>
--- a/Data/suitability_change_output.xlsx
+++ b/Data/suitability_change_output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbouf\Documents\UCSB\Winter 2021\ESM_244\Assignments\amistosa_shiny_app\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E56CA47-83CE-4608-BC9B-4F2BFFD46F72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9562CB9E-A2CC-4632-A32B-C064916241DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-1845" windowWidth="24240" windowHeight="17640" xr2:uid="{EDBCD8E1-F464-4724-B6A6-5FFB702D9B99}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>Time Period</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Suitable Area Gain (hectares)</t>
   </si>
   <si>
-    <t>Net</t>
-  </si>
-  <si>
     <t>Current to 2050 4.5</t>
   </si>
   <si>
@@ -69,31 +66,40 @@
   </si>
   <si>
     <t>Pineapple</t>
+  </si>
+  <si>
+    <t>Net Area Change</t>
+  </si>
+  <si>
+    <t>Suitable Area Gain (Percent)</t>
+  </si>
+  <si>
+    <t>Net Change (percent)</t>
+  </si>
+  <si>
+    <t>Net Change (decimal)</t>
+  </si>
+  <si>
+    <t>Suitable Area Gain (decimal)</t>
+  </si>
+  <si>
+    <t>Suitable Area Lost (decimal)</t>
+  </si>
+  <si>
+    <t>Suitable Area Loss (Percent)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,17 +122,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,233 +438,516 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6235AF86-1BA4-4C68-83A2-87FB82E3148E}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="10" max="10" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C2">
+        <v>1882.6</v>
+      </c>
+      <c r="D2">
+        <v>3850.77</v>
+      </c>
+      <c r="E2">
+        <v>1968.17</v>
+      </c>
+      <c r="F2">
+        <v>3.5400000000000002E-3</v>
+      </c>
+      <c r="G2">
+        <v>7.2300000000000003E-3</v>
+      </c>
+      <c r="H2">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="I2">
+        <f>(F2*100)</f>
+        <v>0.35400000000000004</v>
+      </c>
+      <c r="J2">
+        <f>(G2*100)</f>
+        <v>0.72300000000000009</v>
+      </c>
+      <c r="K2">
+        <f>(H2*100)</f>
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1283.5899999999999</v>
+      </c>
+      <c r="D3">
+        <v>4535.3500000000004</v>
+      </c>
+      <c r="E3">
+        <v>3251.76</v>
+      </c>
+      <c r="F3">
+        <v>2.4099999999999998E-3</v>
+      </c>
+      <c r="G3">
+        <v>8.5199999999999998E-3</v>
+      </c>
+      <c r="H3">
+        <v>6.11E-3</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I13" si="0">(F3*100)</f>
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J13" si="1">(G3*100)</f>
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K13" si="2">(H3*100)</f>
+        <v>0.61099999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1882.6</v>
+      </c>
+      <c r="D4">
+        <v>5391.07</v>
+      </c>
+      <c r="E4">
+        <v>3508.48</v>
+      </c>
+      <c r="F4">
+        <v>3.5300000000000002E-3</v>
+      </c>
+      <c r="G4">
+        <v>1.0120000000000001E-2</v>
+      </c>
+      <c r="H4">
+        <v>6.5900000000000004E-3</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0.35300000000000004</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>1.012</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>0.65900000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>1540.31</v>
+      </c>
+      <c r="D5">
+        <v>2224.89</v>
+      </c>
+      <c r="E5">
+        <v>684.58</v>
+      </c>
+      <c r="F5">
+        <v>2.8900000000000002E-3</v>
+      </c>
+      <c r="G5">
+        <v>4.1799999999999997E-3</v>
+      </c>
+      <c r="H5">
+        <v>1.2800000000000001E-3</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.28900000000000003</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>8300.5400000000009</v>
+      </c>
+      <c r="D6">
+        <v>8728.4</v>
+      </c>
+      <c r="E6">
+        <v>427.86</v>
+      </c>
+      <c r="F6">
+        <v>1.554E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.634E-2</v>
+      </c>
+      <c r="H6">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>1.554</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>1.6340000000000001</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1">
-        <v>1882.6</v>
-      </c>
-      <c r="D2" s="1">
-        <v>3850.77</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1968.17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="C7">
+        <v>5219.93</v>
+      </c>
+      <c r="D7">
+        <v>18398.11</v>
+      </c>
+      <c r="E7">
+        <v>13178.18</v>
+      </c>
+      <c r="F7">
+        <v>9.7699999999999992E-3</v>
+      </c>
+      <c r="G7">
+        <v>3.4439999999999998E-2</v>
+      </c>
+      <c r="H7">
+        <v>2.4670000000000001E-2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0.97699999999999987</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>3.444</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>2.4670000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
-        <v>1283.5899999999999</v>
-      </c>
-      <c r="D3" s="1">
-        <v>4535.3500000000004</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="C8">
+        <v>9070.69</v>
+      </c>
+      <c r="D8">
+        <v>5733.36</v>
+      </c>
+      <c r="E8">
+        <v>-3337.33</v>
+      </c>
+      <c r="F8">
+        <v>1.6979999999999999E-2</v>
+      </c>
+      <c r="G8">
+        <v>1.073E-2</v>
+      </c>
+      <c r="H8">
+        <v>-6.2500000000000003E-3</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1.698</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>1.073</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>-0.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>11124.44</v>
+      </c>
+      <c r="D9">
+        <v>2652.75</v>
+      </c>
+      <c r="E9">
+        <v>-8471.69</v>
+      </c>
+      <c r="F9">
+        <v>2.0830000000000001E-2</v>
+      </c>
+      <c r="G9">
+        <v>4.9699999999999996E-3</v>
+      </c>
+      <c r="H9">
+        <v>-1.5859999999999999E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>2.0830000000000002</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>0.49699999999999994</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>-1.5859999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>4620.92</v>
+      </c>
+      <c r="D10">
+        <v>46465.91</v>
+      </c>
+      <c r="E10">
+        <v>41844.99</v>
+      </c>
+      <c r="F10">
+        <v>8.6499999999999997E-3</v>
+      </c>
+      <c r="G10">
+        <v>8.6989999999999998E-2</v>
+      </c>
+      <c r="H10">
+        <v>7.8340000000000007E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>8.6989999999999998</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>7.8340000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>6417.94</v>
+      </c>
+      <c r="D11">
+        <v>65120.73</v>
+      </c>
+      <c r="E11">
+        <v>58702.79</v>
+      </c>
+      <c r="F11">
+        <v>1.2019999999999999E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.12192</v>
+      </c>
+      <c r="H11">
+        <v>0.1099</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>1.202</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>12.192</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
         <v>3251.76</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="D12">
+        <v>47492.79</v>
+      </c>
+      <c r="E12">
+        <v>44241.03</v>
+      </c>
+      <c r="F12">
+        <v>6.0899999999999999E-3</v>
+      </c>
+      <c r="G12">
+        <v>8.8910000000000003E-2</v>
+      </c>
+      <c r="H12">
+        <v>8.2830000000000001E-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>8.891</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>8.2829999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1882.6</v>
-      </c>
-      <c r="D4" s="1">
-        <v>5391.07</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3508.48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1540.31</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2224.89</v>
-      </c>
-      <c r="E5" s="1">
-        <v>684.58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1">
-        <v>8300.5400000000009</v>
-      </c>
-      <c r="D6" s="1">
-        <v>8728.4</v>
-      </c>
-      <c r="E6" s="1">
-        <v>427.86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1">
-        <v>5219.93</v>
-      </c>
-      <c r="D7" s="1">
-        <v>18398.11</v>
-      </c>
-      <c r="E7" s="1">
-        <v>13178.18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1">
-        <v>9070.69</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5733.36</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-3337.33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1">
-        <v>11124.44</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2652.75</v>
-      </c>
-      <c r="E9" s="1">
-        <v>-8471.69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1">
-        <v>4620.92</v>
-      </c>
-      <c r="D10" s="1">
-        <v>46465.91</v>
-      </c>
-      <c r="E10" s="1">
-        <v>41844.99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6417.94</v>
-      </c>
-      <c r="D11" s="1">
-        <v>65120.73</v>
-      </c>
-      <c r="E11" s="1">
-        <v>58702.79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3251.76</v>
-      </c>
-      <c r="D12" s="1">
-        <v>47492.79</v>
-      </c>
-      <c r="E12" s="1">
-        <v>44241.03</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="42" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>6332.37</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>27297.65</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>20965.28</v>
+      </c>
+      <c r="F13">
+        <v>1.1860000000000001E-2</v>
+      </c>
+      <c r="G13">
+        <v>5.1110000000000003E-2</v>
+      </c>
+      <c r="H13">
+        <v>3.925E-2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>1.1860000000000002</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>5.1110000000000007</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>3.9249999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>